<commit_message>
Updated map script and first version of the dashboard script
</commit_message>
<xml_diff>
--- a/dijon_et_beaune.xlsx
+++ b/dijon_et_beaune.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norsk\dijon_rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4E0394-9491-4814-B191-CE419339FDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1194E595-AD29-440A-AB10-95F1F786417E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-6765" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="1397">
   <si>
     <t>city</t>
   </si>
@@ -4608,8 +4608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF8397E-64F9-4E67-9F19-1F749FE3D23F}">
   <dimension ref="A1:H460"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A423" sqref="A423:XFD423"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7961,8 +7961,8 @@
       <c r="C129" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>395</v>
+      <c r="D129" s="3">
+        <v>21000</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>1341</v>

</xml_diff>